<commit_message>
Commit after Maven build learning
</commit_message>
<xml_diff>
--- a/HybridFramework/TestData/Testdata.xlsx
+++ b/HybridFramework/TestData/Testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91962\eclipse-workspace\HybridFramework\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91962\git\HybridFramework1\HybridFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658CDD69-73FD-490F-8E1C-C4AD47789C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D70358-5213-4CB2-81DB-08558CCFA882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2263" yWindow="2263" windowWidth="16457" windowHeight="9548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>Selenium_50</t>
+    <t>ashish dhaundi</t>
   </si>
   <si>
-    <t>Abcd@123456</t>
+    <t>Nimda@1234</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>